<commit_message>
may dump contents na ung four writers
</commit_message>
<xml_diff>
--- a/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_copy.xlsx
+++ b/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latticesemiconductor4-my.sharepoint.com/personal/jonathan_bunquin_latticesemi_com/Documents/Documents/GitHub/help_dashboard_django/dashboard/online_help/management/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{28E7C28E-CBAD-417D-9B99-6FE99D8518F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE329C26-3AF7-4E0D-B189-7A1FDDEDE7F2}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{28E7C28E-CBAD-417D-9B99-6FE99D8518F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C706BF75-A13F-4230-AECC-8841A6D30A5E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="601" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="online_help_user_guides" sheetId="1" r:id="rId1"/>
@@ -2736,9 +2736,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -4917,7 +4917,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="75" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A107" s="10"/>
       <c r="B107" s="12" t="s">
         <v>63</v>
@@ -6399,7 +6399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912CCFBE-FF25-4E81-B6E7-DB3FD7BFAEC6}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>

</xml_diff>

<commit_message>
edit button in tasks.html
added na rin ang tasks_edit
</commit_message>
<xml_diff>
--- a/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_copy.xlsx
+++ b/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_copy.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latticesemiconductor4-my.sharepoint.com/personal/jonathan_bunquin_latticesemi_com/Documents/Documents/GitHub/help_dashboard_django/dashboard/online_help/management/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{28E7C28E-CBAD-417D-9B99-6FE99D8518F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC2A8ADC-B44B-45E4-B841-B2BC41CC61EF}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{28E7C28E-CBAD-417D-9B99-6FE99D8518F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF31AE7-B9FA-45C3-A90A-D38DFC1118FD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="online_help_user_guides" sheetId="1" r:id="rId1"/>
     <sheet name="online_help_reference" sheetId="5" r:id="rId2"/>
     <sheet name="Standalone_tools_online" sheetId="7" r:id="rId3"/>
     <sheet name="pdf_documents" sheetId="6" r:id="rId4"/>
-    <sheet name="New docs" sheetId="2" r:id="rId5"/>
-    <sheet name="ECNs" sheetId="3" r:id="rId6"/>
+    <sheet name="radiant_docu" sheetId="8" r:id="rId5"/>
+    <sheet name="New docs" sheetId="2" r:id="rId6"/>
+    <sheet name="ECNs" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">online_help_reference!$D$1:$D$43</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="300">
   <si>
     <t>Radiant Documentation</t>
   </si>
@@ -1636,6 +1637,12 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Online Help Reference</t>
+  </si>
+  <si>
+    <t>Standalone Tools</t>
   </si>
 </sst>
 </file>
@@ -2736,7 +2743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -7060,6 +7067,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13D86A2-B61F-40FD-AEDE-2BA08EAA4881}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
@@ -7293,7 +7340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>